<commit_message>
updated export to excel profit and loss reports
</commit_message>
<xml_diff>
--- a/public/extra/export_report/export_report_template_trial_balance.xlsx
+++ b/public/extra/export_report/export_report_template_trial_balance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Classification</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Total Credit</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
   </si>
 </sst>
 </file>
@@ -70,7 +73,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,14 +81,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
@@ -391,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E2"/>
+  <dimension ref="B3:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,21 +419,32 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>